<commit_message>
Excel sheet + IS codes
</commit_message>
<xml_diff>
--- a/data/Cross section properties.xlsx
+++ b/data/Cross section properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IITM\github\Swimminpoollift\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B42D49-E312-47B4-A9D3-734A32EDEDF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2BD0A6-346E-4BCA-9D16-F100E85A0DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18120" yWindow="-15945" windowWidth="18240" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1211,8 +1211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L287"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A244" workbookViewId="0">
-      <selection activeCell="G278" sqref="G278"/>
+    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="M292" sqref="M292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10904,7 +10904,7 @@
         <v>13.6</v>
       </c>
       <c r="H255" s="1">
-        <v>13.6</v>
+        <v>17.3</v>
       </c>
       <c r="I255" s="1">
         <v>325.3</v>
@@ -10942,7 +10942,7 @@
         <v>14.5</v>
       </c>
       <c r="H256" s="1">
-        <v>14.5</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="I256" s="1">
         <v>344.58</v>
@@ -10980,7 +10980,7 @@
         <v>16.2</v>
       </c>
       <c r="H257" s="1">
-        <v>16.2</v>
+        <v>20.6</v>
       </c>
       <c r="I257" s="1">
         <v>382</v>

</xml_diff>